<commit_message>
Fix tests & improve example file
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/with_errors.xlsx
+++ b/src/test/resources/spreadsheets/with_errors.xlsx
@@ -16,7 +16,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>errors</t>
+    <t>amount</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -100,13 +100,16 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,6 +355,14 @@
         <v>#NULL!</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>